<commit_message>
Started coding for enemy
</commit_message>
<xml_diff>
--- a/MI6 Project Plan.xlsx
+++ b/MI6 Project Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lane\MI6\2021FA_SGD285_FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021FA_SGD285_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFAD1A5-BE28-4499-A195-C9F7EAE75D96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FF724B-F86E-4BBA-AFCE-1B405341E267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>Michael &amp; Jennifer</t>
   </si>
   <si>
-    <t>Shared</t>
-  </si>
-  <si>
     <t>Ongoing</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Enemy Destroyed</t>
+  </si>
+  <si>
+    <t>MJZ</t>
   </si>
 </sst>
 </file>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -909,7 +909,7 @@
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="8">
         <v>44524</v>
@@ -1038,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -1125,7 +1125,7 @@
         <v>34</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>3</v>
@@ -1139,7 +1139,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>3</v>
@@ -1147,13 +1147,13 @@
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Project Plan and Level Update
</commit_message>
<xml_diff>
--- a/MI6 Project Plan.xlsx
+++ b/MI6 Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021FA_SGD285_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FF724B-F86E-4BBA-AFCE-1B405341E267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31AC9CE-9AD5-4759-B774-560FAF6F5286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Estimated Implementation</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Michael</t>
   </si>
   <si>
-    <t>FX</t>
-  </si>
-  <si>
     <t>DESIGN</t>
   </si>
   <si>
@@ -162,7 +159,10 @@
     <t>Enemy Destroyed</t>
   </si>
   <si>
-    <t>MJZ</t>
+    <t>MJZ (Zacari)</t>
+  </si>
+  <si>
+    <t>MJZ (Zacari &amp; Michael)</t>
   </si>
 </sst>
 </file>
@@ -682,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -909,7 +909,7 @@
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="8">
         <v>44524</v>
@@ -1038,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -1076,42 +1076,42 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="3"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="8">
-        <v>44524</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
       <c r="B36" s="8"/>
       <c r="C36" s="4"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
+      <c r="B37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>4</v>
@@ -1125,15 +1125,15 @@
         <v>34</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>34</v>
@@ -1142,21 +1142,7 @@
         <v>45</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1199,34 +1185,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D35">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Not Implemented">
-      <formula>NOT(ISERROR(SEARCH("Not Implemented",D30)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D41">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Not Implemented">
-      <formula>NOT(ISERROR(SEARCH("Not Implemented",D36)))</formula>
+  <conditionalFormatting sqref="D35:D40">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",D35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Not Implemented">
+      <formula>NOT(ISERROR(SEARCH("Not Implemented",D35)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -1238,13 +1205,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D22">
-    <cfRule type="containsText" dxfId="2" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="5" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="22" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="4" priority="22" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="23" operator="containsText" text="Not Implemented">
+    <cfRule type="containsText" dxfId="3" priority="23" operator="containsText" text="Not Implemented">
       <formula>NOT(ISERROR(SEARCH("Not Implemented",D8)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -1256,11 +1223,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D30:D34">
+    <cfRule type="containsText" dxfId="2" priority="25" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="26" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="27" operator="containsText" text="Not Implemented">
+      <formula>NOT(ISERROR(SEARCH("Not Implemented",D30)))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B41" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C7:C41" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B40" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C7:C40" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Use the dropdown menu to choose: Not implemented, In Progress or Done." sqref="D3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D41" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D40" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$D$4:$D$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Music and Image added to the menu screen
</commit_message>
<xml_diff>
--- a/MI6 Project Plan.xlsx
+++ b/MI6 Project Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021FA_SGD285_FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrzac\Desktop\285 Software Engineering\GitHub\2021FA_SGD285_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3B5E03-8E7F-47D2-9CE8-929B23C56F60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCEEC77-648B-4353-B3EE-843A68DECA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Estimated Implementation</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Enemies</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Michael</t>
@@ -672,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -808,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -897,7 +894,7 @@
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="8">
         <v>44524</v>
@@ -931,7 +928,7 @@
         <v>44510</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>5</v>
@@ -941,11 +938,11 @@
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>33</v>
+      <c r="B25" s="8">
+        <v>44543</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>3</v>
@@ -959,7 +956,7 @@
         <v>44517</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>5</v>
@@ -1057,7 +1054,7 @@
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="4"/>
@@ -1065,13 +1062,13 @@
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="8">
         <v>44531</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>5</v>
@@ -1079,13 +1076,13 @@
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="8">
         <v>44531</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>5</v>
@@ -1093,7 +1090,7 @@
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="8">
         <v>44531</v>
@@ -1107,13 +1104,13 @@
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="8">
         <v>44531</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>5</v>

</xml_diff>